<commit_message>
Updated "automatic" setting of lambda and kappa
</commit_message>
<xml_diff>
--- a/data/data_source/market_data/commodities-summary-statistics.xlsx
+++ b/data/data_source/market_data/commodities-summary-statistics.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\Documents\git\dynamic-trading\data\data_source\market_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370962A9-0DB9-4724-A2F0-F6D94D6E726B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B716763-FF20-4736-A953-140EEC201062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{49C00968-0AF7-43A3-B5D1-26B7649DFE7B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{49C00968-0AF7-43A3-B5D1-26B7649DFE7B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Correct contract multiplier" sheetId="1" r:id="rId1"/>
+    <sheet name="Simplified contract multiplier" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
     <t>Commodity</t>
   </si>
@@ -93,15 +94,20 @@
   </si>
   <si>
     <t>zinc</t>
+  </si>
+  <si>
+    <t>kappa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -147,7 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -160,6 +166,12 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -477,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C51B1F-E9BD-4EC9-B347-2278894A6D13}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:F14"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="38.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -549,7 +561,7 @@
         <v>5640</v>
       </c>
       <c r="F3" s="4">
-        <f>2*0.1%*B3/(1.59%*E3*C3^2)</f>
+        <f t="shared" ref="F2:F14" si="0">2*0.1%*B3/(1.59%*E3*C3^2)</f>
         <v>1.7812867064860408E-9</v>
       </c>
     </row>
@@ -570,7 +582,7 @@
         <v>12300</v>
       </c>
       <c r="F4" s="4">
-        <f>2*0.1%*B4/(1.59%*E4*C4^2)</f>
+        <f t="shared" si="0"/>
         <v>5.2180118637748467E-7</v>
       </c>
     </row>
@@ -591,7 +603,7 @@
         <v>37260</v>
       </c>
       <c r="F5" s="4">
-        <f>2*0.1%*B5/(1.59%*E5*C5^2)</f>
+        <f t="shared" si="0"/>
         <v>8.7830269141944332E-10</v>
       </c>
     </row>
@@ -612,7 +624,7 @@
         <v>98700</v>
       </c>
       <c r="F6" s="4">
-        <f>2*0.1%*B6/(1.59%*E6*C6^2)</f>
+        <f t="shared" si="0"/>
         <v>3.1419303711024026E-6</v>
       </c>
     </row>
@@ -633,7 +645,7 @@
         <v>2520</v>
       </c>
       <c r="F7" s="4">
-        <f>2*0.1%*B7/(1.59%*E7*C7^2)</f>
+        <f t="shared" si="0"/>
         <v>1.0953557055703977E-5</v>
       </c>
     </row>
@@ -654,7 +666,7 @@
         <v>46120</v>
       </c>
       <c r="F8" s="4">
-        <f>2*0.1%*B8/(1.59%*E8*C8^2)</f>
+        <f t="shared" si="0"/>
         <v>6.0524021587181427E-8</v>
       </c>
     </row>
@@ -675,7 +687,7 @@
         <v>1940</v>
       </c>
       <c r="F9" s="4">
-        <f>2*0.1%*B9/(1.59%*E9*C9^2)</f>
+        <f t="shared" si="0"/>
         <v>4.4421357612557817E-6</v>
       </c>
     </row>
@@ -696,7 +708,7 @@
         <v>43780</v>
       </c>
       <c r="F10" s="4">
-        <f>2*0.1%*B10/(1.59%*E10*C10^2)</f>
+        <f t="shared" si="0"/>
         <v>5.2843868344430649E-9</v>
       </c>
     </row>
@@ -717,7 +729,7 @@
         <v>25700</v>
       </c>
       <c r="F11" s="4">
-        <f>2*0.1%*B11/(1.59%*E11*C11^2)</f>
+        <f t="shared" si="0"/>
         <v>3.9357875653329816E-10</v>
       </c>
     </row>
@@ -738,7 +750,7 @@
         <v>11320</v>
       </c>
       <c r="F12" s="4">
-        <f>2*0.1%*B12/(1.59%*E12*C12^2)</f>
+        <f t="shared" si="0"/>
         <v>3.398996283429756E-7</v>
       </c>
     </row>
@@ -759,7 +771,7 @@
         <v>151160</v>
       </c>
       <c r="F13" s="4">
-        <f>2*0.1%*B13/(1.59%*E13*C13^2)</f>
+        <f t="shared" si="0"/>
         <v>3.4803427326473409E-8</v>
       </c>
     </row>
@@ -780,7 +792,7 @@
         <v>6200</v>
       </c>
       <c r="F14" s="4">
-        <f>2*0.1%*B14/(1.59%*E14*C14^2)</f>
+        <f t="shared" si="0"/>
         <v>2.473487502180431E-6</v>
       </c>
     </row>
@@ -791,4 +803,351 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B6349E-D6B9-4072-A7F4-617C6EEB8C37}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="24.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6328125" style="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2459.8180719061002</v>
+      </c>
+      <c r="C2" s="2">
+        <v>35.987356405301298</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>5320</v>
+      </c>
+      <c r="F2" s="9">
+        <v>4.4908064417933801E-5</v>
+      </c>
+      <c r="G2" s="7">
+        <v>1.2903345408104181E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1771.55670977316</v>
+      </c>
+      <c r="C3" s="2">
+        <v>24.320464537656001</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.15040000000000001</v>
+      </c>
+      <c r="F3" s="8">
+        <v>2.50493443099599</v>
+      </c>
+      <c r="G3" s="7">
+        <v>7.1973786015338895E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>6495.4718753557199</v>
+      </c>
+      <c r="C4" s="2">
+        <v>71.358661932031495</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>492</v>
+      </c>
+      <c r="F4" s="8">
+        <v>3.2612574148592786E-4</v>
+      </c>
+      <c r="G4" s="7">
+        <v>9.3705064856603528E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2">
+        <v>19141.557036423801</v>
+      </c>
+      <c r="C5" s="2">
+        <v>857.75159538895605</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>372.6</v>
+      </c>
+      <c r="F5" s="8">
+        <v>8.7830269141944301E-6</v>
+      </c>
+      <c r="G5" s="7">
+        <v>2.5236097674534401E-7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>42.360101694915201</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.41451292623219094</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>987</v>
+      </c>
+      <c r="F6" s="8">
+        <v>3.1419303711024027E-2</v>
+      </c>
+      <c r="G6" s="7">
+        <v>9.0276464488095876E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2390.35292785192</v>
+      </c>
+      <c r="C7" s="2">
+        <v>20.873707212141799</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>100.8</v>
+      </c>
+      <c r="F7" s="8">
+        <v>6.8459731598149868E-3</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1.9670399399450986E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4.6139496021220099</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.14419304755002299</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4.6120000000000001</v>
+      </c>
+      <c r="F8" s="8">
+        <v>6.0524021587181442</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0.17390247523451094</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2">
+        <v>14828.5271089242</v>
+      </c>
+      <c r="C9" s="2">
+        <v>189.92976879076801</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>323.33333333333331</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1.599168874052082E-4</v>
+      </c>
+      <c r="G9" s="7">
+        <v>4.5948603252521217E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>652.73262518968102</v>
+      </c>
+      <c r="C10" s="2">
+        <v>8.4248836939027303</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>8.7560000000000002</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.13210967086107661</v>
+      </c>
+      <c r="G10" s="7">
+        <v>3.7958810671668156E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2">
+        <v>429.12761132262801</v>
+      </c>
+      <c r="C11" s="2">
+        <v>6.90268837850327</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.2294642857142857</v>
+      </c>
+      <c r="F11" s="8">
+        <v>4.9370519219536915</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0.14185533728163308</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2.0754899176578201</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4.0193289037774402E-2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.2695238095238095</v>
+      </c>
+      <c r="F12" s="8">
+        <v>599.58294439700899</v>
+      </c>
+      <c r="G12" s="7">
+        <v>17.22769826007719</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2">
+        <v>69.178313731985995</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.28609181082494</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>151.16</v>
+      </c>
+      <c r="F13" s="8">
+        <v>3.4803427326473416E-2</v>
+      </c>
+      <c r="G13" s="7">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2691.3448913818602</v>
+      </c>
+      <c r="C14" s="2">
+        <v>29.715319498171201</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>248</v>
+      </c>
+      <c r="F14" s="8">
+        <v>1.5459296888627699E-3</v>
+      </c>
+      <c r="G14" s="7">
+        <v>4.4418892264867501E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added WTI-spot in summary statistics
</commit_message>
<xml_diff>
--- a/data/data_source/market_data/commodities-summary-statistics.xlsx
+++ b/data/data_source/market_data/commodities-summary-statistics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\Documents\git\dynamic-trading\data\data_source\market_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giorgi.POSTEVITA\Documents\ML\dynamic-trading\data\data_source\market_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B716763-FF20-4736-A953-140EEC201062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481124BE-B2DF-484D-B057-88D55E4B9068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{49C00968-0AF7-43A3-B5D1-26B7649DFE7B}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{49C00968-0AF7-43A3-B5D1-26B7649DFE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Correct contract multiplier" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>Commodity</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>kappa</t>
+  </si>
+  <si>
+    <t>WTI-spot</t>
   </si>
 </sst>
 </file>
@@ -104,10 +107,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -151,14 +154,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -166,12 +169,12 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -561,7 +564,7 @@
         <v>5640</v>
       </c>
       <c r="F3" s="4">
-        <f t="shared" ref="F2:F14" si="0">2*0.1%*B3/(1.59%*E3*C3^2)</f>
+        <f t="shared" ref="F3:F14" si="0">2*0.1%*B3/(1.59%*E3*C3^2)</f>
         <v>1.7812867064860408E-9</v>
       </c>
     </row>
@@ -807,10 +810,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B6349E-D6B9-4072-A7F4-617C6EEB8C37}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1146,6 +1149,17 @@
         <v>4.4418892264867501E-5</v>
       </c>
     </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="7">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G15" s="7">
+        <v>1E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added fake_asset and fake_factor
</commit_message>
<xml_diff>
--- a/data/data_source/market_data/commodities-summary-statistics.xlsx
+++ b/data/data_source/market_data/commodities-summary-statistics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giorgi.POSTEVITA\Documents\ML\dynamic-trading\data\data_source\market_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\Documents\git\dynamic-trading\data\data_source\market_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481124BE-B2DF-484D-B057-88D55E4B9068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8AF48D9-11BD-4B9B-AB71-3BA1CCF7B12D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{49C00968-0AF7-43A3-B5D1-26B7649DFE7B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{49C00968-0AF7-43A3-B5D1-26B7649DFE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Correct contract multiplier" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t>Commodity</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>WTI-spot</t>
+  </si>
+  <si>
+    <t>fake_asset</t>
   </si>
 </sst>
 </file>
@@ -107,10 +110,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -154,14 +157,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -169,12 +172,12 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -810,10 +813,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B6349E-D6B9-4072-A7F4-617C6EEB8C37}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1160,6 +1163,17 @@
         <v>1E-3</v>
       </c>
     </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="G16" s="7">
+        <v>0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>